<commit_message>
SUN: iPhone6 reallocation done.
</commit_message>
<xml_diff>
--- a/inventorySheet.xlsx
+++ b/inventorySheet.xlsx
@@ -1586,10 +1586,10 @@
         <v>4444444</v>
       </c>
       <c r="E7" s="13">
-        <v>41274</v>
+        <v>41288</v>
       </c>
       <c r="F7" s="13">
-        <v>41287</v>
+        <v>41304</v>
       </c>
       <c r="G7" t="s" s="11">
         <v>14</v>

</xml_diff>